<commit_message>
Adicionado lógica de execução para carga diária
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephano\Documents\UiPath\GAVB\News\Tech Crunch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4B71C4-E8EF-4514-999A-5AB22035C215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F637DB82-4200-4AAE-8D6F-98D1C4C031D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -252,19 +252,19 @@
     <t>Data da notícia</t>
   </si>
   <si>
+    <t>techcrunch</t>
+  </si>
+  <si>
+    <t>Nome da startup</t>
+  </si>
+  <si>
+    <t>URL_TechCrunch</t>
+  </si>
+  <si>
+    <t>https://search.techcrunch.com/</t>
+  </si>
+  <si>
     <t>True</t>
-  </si>
-  <si>
-    <t>techcrunch</t>
-  </si>
-  <si>
-    <t>Nome da startup</t>
-  </si>
-  <si>
-    <t>URL_TechCrunch</t>
-  </si>
-  <si>
-    <t>https://search.techcrunch.com/</t>
   </si>
 </sst>
 </file>
@@ -685,7 +685,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
         <v>44</v>
@@ -782,7 +782,7 @@
         <v>47</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
         <v>53</v>
@@ -791,10 +791,10 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -803,7 +803,7 @@
         <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1804,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1856,7 +1856,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
#3 início da reestruturação
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephano\Documents\UiPath\GAVB\News\Tech Crunch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F637DB82-4200-4AAE-8D6F-98D1C4C031D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54F4173-9855-4AFE-989B-E0DC0C2EB054}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -244,12 +244,6 @@
   </si>
   <si>
     <t>Carga_Inicial</t>
-  </si>
-  <si>
-    <t>URL da notícia</t>
-  </si>
-  <si>
-    <t>Data da notícia</t>
   </si>
   <si>
     <t>techcrunch</t>
@@ -634,7 +628,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -685,7 +679,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
         <v>44</v>
@@ -759,8 +753,8 @@
       <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>74</v>
+      <c r="B13" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>54</v>
@@ -770,9 +764,7 @@
       <c r="A14" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="B14" s="4"/>
       <c r="C14" t="s">
         <v>53</v>
       </c>
@@ -781,9 +773,7 @@
       <c r="A15" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="B15" s="4"/>
       <c r="C15" t="s">
         <v>53</v>
       </c>
@@ -791,10 +781,10 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -803,7 +793,7 @@
         <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
#3 continuação da reestruturação
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephano\Documents\UiPath\GAVB\News\Tech Crunch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54F4173-9855-4AFE-989B-E0DC0C2EB054}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319196BB-26F2-4A82-B5F3-926B13E7F5FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -628,7 +628,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
#3 estrutura finalizada e adição de lógica carga inicial
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephano\Documents\UiPath\GAVB\News\Tech Crunch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319196BB-26F2-4A82-B5F3-926B13E7F5FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C9D294-C96F-4BFD-832F-AC8DFC568EAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
   <si>
     <t>Name</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>True</t>
+  </si>
+  <si>
+    <t>URL_TechCrunch_Search</t>
+  </si>
+  <si>
+    <t>https://techcrunch.com/</t>
   </si>
 </sst>
 </file>
@@ -625,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -784,19 +790,26 @@
         <v>76</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>73</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1776,12 +1789,13 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{571270CA-D690-4C38-BF0A-B63C6A533FAD}">
       <formula1>"Excel,CSV,TXT"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19" xr:uid="{D000232D-3351-460D-BC2A-631BB9D3640E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20" xr:uid="{D000232D-3351-460D-BC2A-631BB9D3640E}">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1795,7 +1809,7 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1846,7 +1860,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Alteração para rodar carga inicial
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephano\Documents\UiPath\GAVB\News\Tech Crunch\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAEC209-32A5-46EC-9196-A1987F94D197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A9D0FE-FD7C-4B29-9DA8-E11D69FE40D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -264,7 +264,7 @@
     <t>https://techcrunch.com/</t>
   </si>
   <si>
-    <t>False</t>
+    <t>True</t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>